<commit_message>
added J1022 prefold plots, made fit.py run on all *.csv files
</commit_message>
<xml_diff>
--- a/PSC Binary Pulsar Graphs.xlsx
+++ b/PSC Binary Pulsar Graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38300" yWindow="2600" windowWidth="23600" windowHeight="15860" activeTab="1"/>
+    <workbookView xWindow="-38240" yWindow="5120" windowWidth="23600" windowHeight="15860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Epoch (bary) </t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>J1022+101</t>
   </si>
   <si>
     <t>Obs. ID</t>
@@ -65,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">I think this is the right ID, poor quality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think this one was marginial and was excluded </t>
+  </si>
+  <si>
+    <t>J1022+1001</t>
   </si>
 </sst>
 </file>
@@ -158,8 +161,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -183,9 +192,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -241,7 +256,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -402,11 +416,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2100056904"/>
-        <c:axId val="-2100954904"/>
+        <c:axId val="-2125834872"/>
+        <c:axId val="-2125828088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2100056904"/>
+        <c:axId val="-2125834872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,12 +524,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100954904"/>
+        <c:crossAx val="-2125828088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2100954904"/>
+        <c:axId val="-2125828088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,7 +580,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -613,7 +626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100056904"/>
+        <c:crossAx val="-2125834872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -702,7 +715,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -839,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2100872088"/>
-        <c:axId val="-2100865352"/>
+        <c:axId val="-2125752568"/>
+        <c:axId val="-2125745928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2100872088"/>
+        <c:axId val="-2125752568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +901,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -936,12 +947,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100865352"/>
+        <c:crossAx val="-2125745928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2100865352"/>
+        <c:axId val="-2125745928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1003,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1039,7 +1049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100872088"/>
+        <c:crossAx val="-2125752568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1128,7 +1138,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1271,11 +1280,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2100823256"/>
-        <c:axId val="-2100816520"/>
+        <c:axId val="-2125703736"/>
+        <c:axId val="-2125697096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2100823256"/>
+        <c:axId val="-2125703736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1330,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1368,12 +1376,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100816520"/>
+        <c:crossAx val="-2125697096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2100816520"/>
+        <c:axId val="-2125697096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1424,7 +1432,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1471,7 +1478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100823256"/>
+        <c:crossAx val="-2125703736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1698,11 +1705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2100747800"/>
-        <c:axId val="-2100744088"/>
+        <c:axId val="-2125624312"/>
+        <c:axId val="-2125620600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2100747800"/>
+        <c:axId val="-2125624312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1759,12 +1766,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100744088"/>
+        <c:crossAx val="-2125620600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2100744088"/>
+        <c:axId val="-2125620600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,7 +1828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100747800"/>
+        <c:crossAx val="-2125624312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4483,7 +4490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4662,7 +4669,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4939,30 +4946,30 @@
     </row>
     <row r="14" spans="1:13">
       <c r="G14" s="7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1">
       <c r="G15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="J15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="K15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="M15" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1">
@@ -5202,7 +5209,7 @@
         <v>16.451579519999999</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21">
         <v>22990</v>
@@ -5229,7 +5236,7 @@
         <v>4.3000000000000003E-6</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" thickBot="1">
@@ -5251,6 +5258,9 @@
       <c r="E22" s="4">
         <v>16.456319000000001</v>
       </c>
+      <c r="G22">
+        <v>29213</v>
+      </c>
       <c r="H22" s="6">
         <v>57949.012219999997</v>
       </c>
@@ -5268,6 +5278,9 @@
       </c>
       <c r="L22" s="4">
         <v>5.3623209599999999</v>
+      </c>
+      <c r="M22">
+        <v>4.8999999999999997E-6</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15" thickBot="1">
@@ -5301,8 +5314,14 @@
         <v>29.050242616033614</v>
       </c>
       <c r="L23" s="4"/>
+      <c r="N23" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ht="15" thickBot="1">
+      <c r="G24">
+        <v>29303</v>
+      </c>
       <c r="H24" s="5">
         <v>57949.070639999998</v>
       </c>
@@ -5321,8 +5340,14 @@
       <c r="L24" s="4">
         <v>5.3623209599999999</v>
       </c>
+      <c r="M24">
+        <v>4.1999999999999996E-6</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="15" thickBot="1">
+      <c r="G25">
+        <v>29296</v>
+      </c>
       <c r="H25" s="1">
         <v>57949.2601</v>
       </c>
@@ -5340,6 +5365,9 @@
       </c>
       <c r="L25" s="4">
         <v>5.3623295999999998</v>
+      </c>
+      <c r="M25">
+        <v>1.1999999999999999E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added J2145, removed spaces in .txt output
</commit_message>
<xml_diff>
--- a/PSC Binary Pulsar Graphs.xlsx
+++ b/PSC Binary Pulsar Graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38240" yWindow="5120" windowWidth="23600" windowHeight="15860" activeTab="1"/>
+    <workbookView xWindow="3000" yWindow="880" windowWidth="23600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Epoch (bary) </t>
   </si>
@@ -55,9 +55,6 @@
     <t>Period corrected to Barry</t>
   </si>
   <si>
-    <t>Uncorreceted Period Error</t>
-  </si>
-  <si>
     <t>Might be wrong uncorreted error, two points on mjd</t>
   </si>
   <si>
@@ -68,6 +65,24 @@
   </si>
   <si>
     <t>J1022+1001</t>
+  </si>
+  <si>
+    <t>Topo Period Error</t>
+  </si>
+  <si>
+    <t>J2145-0750</t>
+  </si>
+  <si>
+    <t>Topo Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay Period </t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>ID (My best guess)</t>
   </si>
 </sst>
 </file>
@@ -161,8 +176,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -192,15 +211,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -256,6 +279,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -416,11 +440,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125834872"/>
-        <c:axId val="-2125828088"/>
+        <c:axId val="-2103975224"/>
+        <c:axId val="-2104126040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125834872"/>
+        <c:axId val="-2103975224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,12 +548,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125828088"/>
+        <c:crossAx val="-2104126040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125828088"/>
+        <c:axId val="-2104126040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,6 +604,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -626,7 +651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125834872"/>
+        <c:crossAx val="-2103975224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -715,6 +740,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -772,7 +798,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$16:$D$23</c:f>
+              <c:f>Sheet2!$E$16:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -805,7 +831,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$E$16:$E$23</c:f>
+              <c:f>Sheet2!$F$16:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -851,11 +877,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125752568"/>
-        <c:axId val="-2125745928"/>
+        <c:axId val="-2104443336"/>
+        <c:axId val="-2103503960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125752568"/>
+        <c:axId val="-2104443336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,6 +927,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -947,12 +974,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125745928"/>
+        <c:crossAx val="-2103503960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125745928"/>
+        <c:axId val="-2103503960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,6 +1030,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1049,7 +1077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125752568"/>
+        <c:crossAx val="-2104443336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1138,6 +1166,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1195,7 +1224,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$K$16:$K$25</c:f>
+              <c:f>Sheet2!$M$16:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1231,7 +1260,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$L$16:$L$25</c:f>
+              <c:f>Sheet2!$N$16:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1280,11 +1309,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125703736"/>
-        <c:axId val="-2125697096"/>
+        <c:axId val="2105218984"/>
+        <c:axId val="2105229848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125703736"/>
+        <c:axId val="2105218984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,6 +1359,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1376,12 +1406,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125697096"/>
+        <c:crossAx val="2105229848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125697096"/>
+        <c:axId val="2105229848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,6 +1462,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1478,7 +1509,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125703736"/>
+        <c:crossAx val="2105218984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1620,7 +1651,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$K$16:$K$25</c:f>
+              <c:f>Sheet2!$M$16:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1656,7 +1687,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$L$16:$L$25</c:f>
+              <c:f>Sheet2!$N$16:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1705,11 +1736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125624312"/>
-        <c:axId val="-2125620600"/>
+        <c:axId val="2105403048"/>
+        <c:axId val="2105406824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125624312"/>
+        <c:axId val="2105403048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,12 +1797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125620600"/>
+        <c:crossAx val="2105406824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125620600"/>
+        <c:axId val="2105406824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,7 +1859,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125624312"/>
+        <c:crossAx val="2105403048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4204,13 +4235,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>471487</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>92075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>166687</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -4490,7 +4521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4666,713 +4697,780 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="1">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
+      <c r="B1" s="1">
         <v>57602.502840000001</v>
       </c>
-      <c r="B1">
-        <f>A1-$A$1</f>
+      <c r="C1">
+        <f>B1-$B$1</f>
         <v>0</v>
       </c>
-      <c r="C1">
-        <f>B1/5.74</f>
+      <c r="D1">
+        <f>C1/5.74</f>
         <v>0</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>0</v>
       </c>
-      <c r="K1">
+      <c r="M1">
         <v>0</v>
       </c>
-      <c r="L1" s="4">
+      <c r="N1" s="4">
         <v>5.7575366199999998</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1">
-      <c r="A2" s="1">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
+      <c r="B2" s="1">
         <v>57603.533159999999</v>
       </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B12" si="0">A2-$A$1</f>
+      <c r="C2">
+        <f t="shared" ref="C2:C12" si="0">B2-$B$1</f>
         <v>1.0303199999980279</v>
       </c>
-      <c r="C2">
-        <f>B2/5.74</f>
+      <c r="D2">
+        <f>C2/5.74</f>
         <v>0.17949825783937767</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.17949799999999999</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>0.17949799999999999</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>5.7573899400000004</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
-      <c r="A3" s="3">
+    <row r="3" spans="1:15" ht="15" thickBot="1">
+      <c r="B3" s="3">
         <v>57946.564769999997</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <f t="shared" si="0"/>
         <v>344.06192999999621</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C12" si="1">B3/5.74</f>
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="1">C3/5.74</f>
         <v>59.941102787455783</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.94110000000000005</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>0.94110000000000005</v>
       </c>
-      <c r="L3" s="3">
+      <c r="N3" s="3">
         <v>5.7576472299999999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1">
-      <c r="A4" s="3">
+    <row r="4" spans="1:15" ht="15" thickBot="1">
+      <c r="B4" s="3">
         <v>57946.598510000003</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <f t="shared" si="0"/>
         <v>344.09567000000243</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <f t="shared" si="1"/>
         <v>59.946980836237351</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.94698000000000004</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>0.94698000000000004</v>
       </c>
-      <c r="L4" s="3">
+      <c r="N4" s="3">
         <v>5.7576470100000003</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1">
-      <c r="A5" s="3">
+    <row r="5" spans="1:15" ht="15" thickBot="1">
+      <c r="B5" s="3">
         <v>57947.589870000003</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>345.08703000000241</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <f t="shared" si="1"/>
         <v>60.119691637631078</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.11969</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>0.11969</v>
       </c>
-      <c r="L5" s="3">
+      <c r="N5" s="3">
         <v>5.7574294300000002</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1">
-      <c r="A6" s="3">
+    <row r="6" spans="1:15" ht="15" thickBot="1">
+      <c r="B6" s="3">
         <v>57947.606169999999</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>345.1033299999981</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <f t="shared" si="1"/>
         <v>60.122531358884686</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.12253</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>0.12253</v>
       </c>
-      <c r="L6" s="3">
+      <c r="N6" s="3">
         <v>5.7574242699999996</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
-      <c r="A7" s="3">
+    <row r="7" spans="1:15" ht="15" thickBot="1">
+      <c r="B7" s="3">
         <v>57947.609920000003</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>345.10708000000159</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <f t="shared" si="1"/>
         <v>60.123184668989822</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.12318</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>0.12318</v>
       </c>
-      <c r="L7" s="3">
+      <c r="N7" s="3">
         <v>5.7574155100000004</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1">
-      <c r="A8" s="3">
+    <row r="8" spans="1:15" ht="15" thickBot="1">
+      <c r="B8" s="3">
         <v>57947.613669999999</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>345.1108299999978</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <f t="shared" si="1"/>
         <v>60.123837979093693</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.12384000000000001</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>0.12384000000000001</v>
       </c>
-      <c r="L8" s="3">
+      <c r="N8" s="3">
         <v>5.7574222700000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
-      <c r="A9" s="3">
+    <row r="9" spans="1:15" ht="15" thickBot="1">
+      <c r="B9" s="3">
         <v>57947.617440000002</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>345.11460000000079</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <f t="shared" si="1"/>
         <v>60.124494773519302</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.12449</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>0.12449</v>
       </c>
-      <c r="L9" s="3">
+      <c r="N9" s="3">
         <v>5.7574225500000002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1">
-      <c r="A10" s="1">
+    <row r="10" spans="1:15" ht="15" thickBot="1">
+      <c r="B10" s="1">
         <v>57948.57804</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>346.07519999999931</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <f t="shared" si="1"/>
         <v>60.291846689895351</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.29185</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>0.29185</v>
       </c>
-      <c r="L10" s="2">
+      <c r="N10" s="2">
         <v>5.7572221600000004</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1">
-      <c r="A11" s="1">
+    <row r="11" spans="1:15" ht="15" thickBot="1">
+      <c r="B11" s="1">
         <v>57948.590859999997</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>346.08801999999559</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <f t="shared" si="1"/>
         <v>60.294080139372049</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.29408000000000001</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>0.29408000000000001</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N11" s="2">
         <v>5.7572245999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1">
-      <c r="A12" s="1">
+    <row r="12" spans="1:15" ht="15" thickBot="1">
+      <c r="B12" s="1">
         <v>57949.552989999996</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>347.05014999999548</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <f t="shared" si="1"/>
         <v>60.461698606270986</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.4617</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>0.4617</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1">
         <v>5.7572380000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="G14" s="7" t="s">
+    <row r="14" spans="1:15">
+      <c r="I14" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1">
+      <c r="A15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
-      <c r="G15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>10</v>
+    <row r="16" spans="1:15" ht="15" thickBot="1">
+      <c r="A16">
+        <v>22517</v>
+      </c>
+      <c r="B16" s="3">
+        <v>57590.617619999997</v>
+      </c>
+      <c r="C16">
+        <f>B16-$B$16</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>C16/7.805</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>16.45347168</v>
+      </c>
+      <c r="G16">
+        <v>8.3000000000000002E-6</v>
+      </c>
+      <c r="I16">
+        <v>22570</v>
+      </c>
+      <c r="J16" s="6">
+        <v>57591.00434</v>
+      </c>
+      <c r="K16">
+        <f>J16-$J$16</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>K16/12.324</f>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>5.3623209599999999</v>
+      </c>
+      <c r="O16">
+        <v>8.8000000000000004E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1">
-      <c r="A16" s="3">
-        <v>57590.617619999997</v>
-      </c>
-      <c r="B16">
-        <f>A16-$A$16</f>
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <f>B16/7.805</f>
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>16.45347168</v>
-      </c>
-      <c r="G16">
-        <v>22570</v>
-      </c>
-      <c r="H16" s="6">
-        <v>57591.00434</v>
-      </c>
-      <c r="I16">
-        <f>H16-$H$16</f>
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <f>I16/12.324</f>
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <v>5.3623209599999999</v>
-      </c>
-      <c r="M16">
-        <v>8.8000000000000004E-7</v>
+    <row r="17" spans="1:16" ht="15" thickBot="1">
+      <c r="A17">
+        <v>22696</v>
+      </c>
+      <c r="B17" s="3">
+        <v>57595.620389999996</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:C23" si="2">B17-$B$16</f>
+        <v>5.0027699999991455</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D23" si="3">C17/7.805</f>
+        <v>0.64096989109534219</v>
+      </c>
+      <c r="E17">
+        <f>D17-0</f>
+        <v>0.64096989109534219</v>
+      </c>
+      <c r="F17" s="4">
+        <v>16.4541024</v>
+      </c>
+      <c r="G17" s="4">
+        <v>4.4000000000000002E-6</v>
+      </c>
+      <c r="I17">
+        <v>22697</v>
+      </c>
+      <c r="J17" s="6">
+        <v>57595.978109999996</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17:K21" si="4">J17-$J$16</f>
+        <v>4.9737699999968754</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17:L21" si="5">K17/12.324</f>
+        <v>0.40358406361545568</v>
+      </c>
+      <c r="M17">
+        <f>L17</f>
+        <v>0.40358406361545568</v>
+      </c>
+      <c r="N17" s="4">
+        <v>5.3616988799999996</v>
+      </c>
+      <c r="O17">
+        <v>3.4000000000000001E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1">
-      <c r="A17" s="3">
-        <v>57595.620389999996</v>
-      </c>
-      <c r="B17">
-        <f t="shared" ref="B17:B23" si="2">A17-$A$16</f>
-        <v>5.0027699999991455</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ref="C17:C23" si="3">B17/7.805</f>
-        <v>0.64096989109534219</v>
-      </c>
-      <c r="D17">
-        <f>C17-0</f>
-        <v>0.64096989109534219</v>
-      </c>
-      <c r="E17" s="4">
-        <v>16.4541024</v>
-      </c>
-      <c r="G17">
-        <v>22697</v>
-      </c>
-      <c r="H17" s="6">
-        <v>57595.978109999996</v>
-      </c>
-      <c r="I17">
-        <f t="shared" ref="I17:I21" si="4">H17-$H$16</f>
-        <v>4.9737699999968754</v>
-      </c>
-      <c r="J17">
-        <f t="shared" ref="J17:J21" si="5">I17/12.324</f>
-        <v>0.40358406361545568</v>
-      </c>
-      <c r="K17">
-        <f>J17</f>
-        <v>0.40358406361545568</v>
-      </c>
-      <c r="L17" s="4">
-        <v>5.3616988799999996</v>
-      </c>
-      <c r="M17">
-        <v>3.4000000000000001E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1">
-      <c r="A18" s="3">
+    <row r="18" spans="1:16" ht="15" thickBot="1">
+      <c r="A18">
+        <v>22739</v>
+      </c>
+      <c r="B18" s="3">
         <v>57596.679779999999</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <f t="shared" si="2"/>
         <v>6.0621600000013132</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <f t="shared" si="3"/>
         <v>0.77670211402963651</v>
       </c>
-      <c r="D18">
-        <f>C18-0</f>
+      <c r="E18">
+        <f>D18-0</f>
         <v>0.77670211402963651</v>
       </c>
-      <c r="E18" s="4">
+      <c r="F18" s="4">
         <v>16.4553552</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="4">
+        <v>3.4000000000000001E-6</v>
+      </c>
+      <c r="I18">
         <v>22759</v>
       </c>
-      <c r="H18" s="6">
+      <c r="J18" s="6">
         <v>57596.967830000001</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <f t="shared" si="4"/>
         <v>5.9634900000019115</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <f t="shared" si="5"/>
         <v>0.48389240506344627</v>
       </c>
-      <c r="K18">
-        <f>J18</f>
+      <c r="M18">
+        <f>L18</f>
         <v>0.48389240506344627</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>5.3616902399999997</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1">
-      <c r="A19" s="3">
+    <row r="19" spans="1:16" ht="15" thickBot="1">
+      <c r="A19">
+        <v>22827</v>
+      </c>
+      <c r="B19" s="3">
         <v>57598.636050000001</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <f t="shared" si="2"/>
         <v>8.0184300000037183</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <f t="shared" si="3"/>
         <v>1.027345291480297</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>2.7345000000000001E-2</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>16.454093759999999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="4">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="I19">
         <v>22826</v>
       </c>
-      <c r="H19" s="6">
+      <c r="J19" s="6">
         <v>57598.962399999997</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <f t="shared" si="4"/>
         <v>7.9580599999972037</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <f t="shared" si="5"/>
         <v>0.64573677377452154</v>
       </c>
-      <c r="K19">
-        <f>J19</f>
+      <c r="M19">
+        <f>L19</f>
         <v>0.64573677377452154</v>
       </c>
-      <c r="L19" s="4">
+      <c r="N19" s="4">
         <v>5.3610681600000003</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>6.1999999999999999E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1">
-      <c r="A20" s="3">
+    <row r="20" spans="1:16" ht="15" thickBot="1">
+      <c r="A20">
+        <v>22903</v>
+      </c>
+      <c r="B20" s="3">
         <v>57601.745770000001</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <f t="shared" si="2"/>
         <v>11.128150000004098</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <f t="shared" si="3"/>
         <v>1.425771941063946</v>
       </c>
-      <c r="D20">
-        <f>C20-1</f>
+      <c r="E20">
+        <f>D20-1</f>
         <v>0.425771941063946</v>
       </c>
-      <c r="E20" s="4">
+      <c r="F20" s="4">
         <v>16.450948799999999</v>
       </c>
       <c r="G20">
+        <v>6.1999999999999999E-6</v>
+      </c>
+      <c r="I20">
         <v>22904</v>
       </c>
-      <c r="H20" s="6">
+      <c r="J20" s="6">
         <v>57601.918440000001</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <f t="shared" si="4"/>
         <v>10.914100000001781</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <f t="shared" si="5"/>
         <v>0.88559720869861902</v>
       </c>
-      <c r="K20">
-        <f>J20</f>
+      <c r="M20">
+        <f>L20</f>
         <v>0.88559720869861902</v>
       </c>
-      <c r="L20" s="4">
+      <c r="N20" s="4">
         <v>5.3616988799999996</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>4.1999999999999996E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1">
-      <c r="A21" s="3">
+    <row r="21" spans="1:16" ht="15" thickBot="1">
+      <c r="A21">
+        <v>29138</v>
+      </c>
+      <c r="B21" s="3">
         <v>57945.926050000002</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <f t="shared" si="2"/>
         <v>355.30843000000459</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <f t="shared" si="3"/>
         <v>45.523181294042871</v>
       </c>
-      <c r="D21">
-        <f>C21-45</f>
+      <c r="E21">
+        <f>D21-45</f>
         <v>0.52318129404287106</v>
       </c>
-      <c r="E21" s="4">
+      <c r="F21" s="4">
         <v>16.451579519999999</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21">
+      <c r="G21" s="4">
+        <v>4.3000000000000003E-6</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21">
         <v>22990</v>
       </c>
-      <c r="H21" s="6">
+      <c r="J21" s="6">
         <v>57603.145479999999</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <f t="shared" si="4"/>
         <v>12.141139999999723</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <f t="shared" si="5"/>
         <v>0.98516228497238911</v>
       </c>
-      <c r="K21">
-        <f>J21</f>
+      <c r="M21">
+        <f>L21</f>
         <v>0.98516228497238911</v>
       </c>
-      <c r="L21" s="4">
+      <c r="N21" s="4">
         <v>5.3629516800000001</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>4.3000000000000003E-6</v>
       </c>
-      <c r="N21" s="7" t="s">
-        <v>11</v>
+      <c r="P21" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1">
-      <c r="A22" s="3">
+    <row r="22" spans="1:16" ht="15" thickBot="1">
+      <c r="A22">
+        <v>29236</v>
+      </c>
+      <c r="B22" s="3">
         <v>57948.641519999997</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <f t="shared" si="2"/>
         <v>358.02390000000014</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <f t="shared" si="3"/>
         <v>45.871095451633586</v>
       </c>
-      <c r="D22">
-        <f>C22-45</f>
+      <c r="E22">
+        <f>D22-45</f>
         <v>0.87109545163358604</v>
       </c>
-      <c r="E22" s="4">
+      <c r="F22" s="4">
         <v>16.456319000000001</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="4">
+        <v>4.6999999999999999E-6</v>
+      </c>
+      <c r="I22">
         <v>29213</v>
       </c>
-      <c r="H22" s="6">
+      <c r="J22" s="6">
         <v>57949.012219999997</v>
       </c>
-      <c r="I22">
-        <f>H22-$H$16</f>
+      <c r="K22">
+        <f>J22-$J$16</f>
         <v>358.00787999999739</v>
       </c>
-      <c r="J22">
-        <f>I22/12.324</f>
+      <c r="L22">
+        <f>K22/12.324</f>
         <v>29.049649464459378</v>
       </c>
-      <c r="K22">
-        <f>J22-29</f>
+      <c r="M22">
+        <f>L22-29</f>
         <v>4.9649464459378123E-2</v>
       </c>
-      <c r="L22" s="4">
+      <c r="N22" s="4">
         <v>5.3623209599999999</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>4.8999999999999997E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1">
-      <c r="A23" s="3">
+    <row r="23" spans="1:16" ht="15" thickBot="1">
+      <c r="A23">
+        <v>29298</v>
+      </c>
+      <c r="B23" s="3">
         <v>57948.736859999997</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <f t="shared" si="2"/>
         <v>358.11923999999999</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <f t="shared" si="3"/>
         <v>45.883310698270343</v>
       </c>
-      <c r="D23">
-        <f>C23-45</f>
+      <c r="E23">
+        <f>D23-45</f>
         <v>0.8833106982703427</v>
       </c>
-      <c r="E23" s="4">
+      <c r="F23" s="4">
         <v>16.455346559999999</v>
       </c>
-      <c r="H23" s="1">
+      <c r="G23" s="4">
+        <v>2.7E-6</v>
+      </c>
+      <c r="J23" s="1">
         <v>57949.019529999998</v>
       </c>
-      <c r="I23">
-        <f>H23-$H$16</f>
+      <c r="K23">
+        <f>J23-$J$16</f>
         <v>358.01518999999826</v>
       </c>
-      <c r="J23">
-        <f>I23/12.324</f>
+      <c r="L23">
+        <f>K23/12.324</f>
         <v>29.050242616033614</v>
       </c>
-      <c r="L23" s="4"/>
-      <c r="N23" s="7" t="s">
-        <v>13</v>
+      <c r="N23" s="4"/>
+      <c r="P23" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1">
-      <c r="G24">
+    <row r="24" spans="1:16" ht="15" thickBot="1">
+      <c r="I24">
         <v>29303</v>
       </c>
-      <c r="H24" s="5">
+      <c r="J24" s="5">
         <v>57949.070639999998</v>
       </c>
-      <c r="I24">
-        <f>H24-$H$16</f>
+      <c r="K24">
+        <f>J24-$J$16</f>
         <v>358.06629999999859</v>
       </c>
-      <c r="J24">
-        <f>I24/12.324</f>
+      <c r="L24">
+        <f>K24/12.324</f>
         <v>29.054389808503618</v>
       </c>
-      <c r="K24">
-        <f>J24-29</f>
+      <c r="M24">
+        <f>L24-29</f>
         <v>5.4389808503618298E-2</v>
       </c>
-      <c r="L24" s="4">
+      <c r="N24" s="4">
         <v>5.3623209599999999</v>
       </c>
-      <c r="M24">
+      <c r="O24">
         <v>4.1999999999999996E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1">
-      <c r="G25">
+    <row r="25" spans="1:16" ht="15" thickBot="1">
+      <c r="I25">
         <v>29296</v>
       </c>
-      <c r="H25" s="1">
+      <c r="J25" s="1">
         <v>57949.2601</v>
       </c>
-      <c r="I25">
-        <f>H25-$H$16</f>
+      <c r="K25">
+        <f>J25-$J$16</f>
         <v>358.25576000000001</v>
       </c>
-      <c r="J25">
-        <f>I25/12.324</f>
+      <c r="L25">
+        <f>K25/12.324</f>
         <v>29.069763063940279</v>
       </c>
-      <c r="K25">
-        <f>J25-29</f>
+      <c r="M25">
+        <f>L25-29</f>
         <v>6.9763063940278869E-2</v>
       </c>
-      <c r="L25" s="4">
+      <c r="N25" s="4">
         <v>5.3623295999999998</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>1.1999999999999999E-6</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="H16:H30">
-    <sortCondition ref="H16:H30"/>
+  <sortState ref="J16:J30">
+    <sortCondition ref="J16:J30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>